<commit_message>
FEAT: 9618_s24_42 and 9618_s24_43
</commit_message>
<xml_diff>
--- a/Task Update.xlsx
+++ b/Task Update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Data\P4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366BD621-436C-4118-B379-912640A27043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A9DB40-9360-492D-A74C-E6613CAB004E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>S.No.</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>9618_s21_43</t>
+  </si>
+  <si>
+    <t>9618_s24_43</t>
+  </si>
+  <si>
+    <t>9618_s24_42</t>
   </si>
 </sst>
 </file>
@@ -429,7 +435,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,13 +514,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -522,13 +522,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -536,9 +530,12 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -547,10 +544,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -558,7 +558,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -569,23 +569,35 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FIX: 9618_s24_41 evidence doc and other files
</commit_message>
<xml_diff>
--- a/Task Update.xlsx
+++ b/Task Update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Data\P4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A9DB40-9360-492D-A74C-E6613CAB004E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45D8791-8608-41EA-B238-7B049E956FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>S.No.</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Incomplete</t>
-  </si>
-  <si>
-    <t>Evidence doc and text file needs to be uploaded</t>
   </si>
   <si>
     <t>Complete</t>
@@ -435,7 +432,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +484,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -495,7 +492,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -505,16 +502,13 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -522,7 +516,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -572,7 +566,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
9618_s24_41 Question 1 completed by Suhair Pasta
</commit_message>
<xml_diff>
--- a/Task Update.xlsx
+++ b/Task Update.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Data\P4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Highbrow Students\Music\ammar hacker\CS-P4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45D8791-8608-41EA-B238-7B049E956FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3877BF58-C94B-41CF-8FFF-1387B1DB0110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P4" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>S.No.</t>
   </si>
@@ -432,7 +432,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,6 +502,9 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">

</xml_diff>